<commit_message>
Added figures of co-sim and frequency response
</commit_message>
<xml_diff>
--- a/pct/modules/06/network_model/ieee14_full.xlsx
+++ b/pct/modules/06/network_model/ieee14_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfang\gitrepos\andes\andes\cases\ieee14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb1052\Desktop\powercybertraining.github.io\pct\modules\06\network_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3F7360BD-A95E-46DF-96B4-69FB6C6744A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C1C3CBC-A3CA-457F-9C9D-492924F08749}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BB5486-8D61-498D-B3D7-17C882068C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="552" windowWidth="18336" windowHeight="11436" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="BusFreq" sheetId="16" r:id="rId16"/>
     <sheet name="ACEc" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="209">
   <si>
     <t>uid</t>
   </si>
@@ -671,13 +671,16 @@
   </si>
   <si>
     <t>ACE_1</t>
+  </si>
+  <si>
+    <t>BusFreq_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,7 +705,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -725,13 +728,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1079,9 +1096,9 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1169,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1213,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1257,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1301,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1345,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1389,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1433,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1477,7 +1494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1521,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1565,7 +1582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1609,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1653,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1697,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1755,9 +1772,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1818,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1842,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1883,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1938,9 +1955,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2026,7 +2043,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2106,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2200,9 +2217,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2272,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2322,9 +2339,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2421,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2484,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2564,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2738,9 +2755,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2834,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2905,9 +2922,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2990,7 +3007,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3067,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3151,16 +3168,16 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3186,7 +3203,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3212,7 +3229,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3238,7 +3255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3261,6 +3278,32 @@
         <v>0.02</v>
       </c>
       <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
+      </c>
+      <c r="H5">
         <v>60</v>
       </c>
     </row>
@@ -3274,13 +3317,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="G2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3303,7 +3346,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>1</v>
       </c>
@@ -3334,9 +3377,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3371,7 +3414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3406,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3441,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3476,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3511,7 +3554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3546,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3581,7 +3624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3616,7 +3659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3651,7 +3694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3686,7 +3729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3721,7 +3764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3770,9 +3813,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3831,7 +3874,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3887,7 +3930,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3943,7 +3986,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3999,7 +4042,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4069,9 +4112,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4133,7 +4176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4206,9 +4249,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4283,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4272,7 +4315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4318,9 +4361,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4394,7 +4437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4459,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4524,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4589,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4654,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4719,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4784,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4849,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4914,7 +4957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4979,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5044,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5109,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5174,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5239,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5304,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5369,7 +5412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5434,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5499,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5564,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5629,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5708,9 +5751,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5724,7 +5767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5738,7 +5781,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5766,9 +5809,9 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5791,10 +5834,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
@@ -5811,9 +5854,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5899,7 +5942,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5982,7 +6025,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6065,7 +6108,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6148,7 +6191,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6231,7 +6274,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Merge latest changes from MSU.
</commit_message>
<xml_diff>
--- a/pct/modules/06/network_model/ieee14_full.xlsx
+++ b/pct/modules/06/network_model/ieee14_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfang\gitrepos\andes\andes\cases\ieee14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb1052\Desktop\powercybertraining.github.io\pct\modules\06\network_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3F7360BD-A95E-46DF-96B4-69FB6C6744A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C1C3CBC-A3CA-457F-9C9D-492924F08749}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BB5486-8D61-498D-B3D7-17C882068C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="552" windowWidth="18336" windowHeight="11436" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="BusFreq" sheetId="16" r:id="rId16"/>
     <sheet name="ACEc" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="209">
   <si>
     <t>uid</t>
   </si>
@@ -671,13 +671,16 @@
   </si>
   <si>
     <t>ACE_1</t>
+  </si>
+  <si>
+    <t>BusFreq_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,7 +705,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -725,13 +728,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1079,9 +1096,9 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1169,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1213,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1257,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1301,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1345,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1389,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1433,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1477,7 +1494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1521,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1565,7 +1582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1609,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1653,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1697,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1755,9 +1772,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1818,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1842,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1883,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1938,9 +1955,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2026,7 +2043,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2106,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2200,9 +2217,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2272,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2322,9 +2339,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2421,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2484,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2564,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2738,9 +2755,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2834,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2905,9 +2922,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2990,7 +3007,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3067,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3151,16 +3168,16 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3186,7 +3203,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3212,7 +3229,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3238,7 +3255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3261,6 +3278,32 @@
         <v>0.02</v>
       </c>
       <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
+      </c>
+      <c r="H5">
         <v>60</v>
       </c>
     </row>
@@ -3274,13 +3317,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="G2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3303,7 +3346,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>1</v>
       </c>
@@ -3334,9 +3377,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3371,7 +3414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3406,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3441,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3476,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3511,7 +3554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3546,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3581,7 +3624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3616,7 +3659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3651,7 +3694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3686,7 +3729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3721,7 +3764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3770,9 +3813,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3831,7 +3874,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3887,7 +3930,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3943,7 +3986,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3999,7 +4042,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4069,9 +4112,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4133,7 +4176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4206,9 +4249,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4283,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4272,7 +4315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4318,9 +4361,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4394,7 +4437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4459,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4524,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4589,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4654,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4719,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4784,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4849,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4914,7 +4957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4979,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5044,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5109,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5174,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5239,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5304,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5369,7 +5412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5434,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5499,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5564,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5629,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5708,9 +5751,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5724,7 +5767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5738,7 +5781,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5766,9 +5809,9 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5791,10 +5834,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
@@ -5811,9 +5854,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5899,7 +5942,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5982,7 +6025,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6065,7 +6108,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6148,7 +6191,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6231,7 +6274,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>

</xml_diff>